<commit_message>
changed ISA to be 8 bit instead of 4 bit
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSCE312Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70CD4CD-7402-4078-A952-5F8B9CD84CAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2917928D-D673-4BDC-A321-6D27F88DB423}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,22 +75,22 @@
     <t>return</t>
   </si>
   <si>
-    <t>Dest (4)</t>
-  </si>
-  <si>
     <t>rA</t>
   </si>
   <si>
     <t>rB</t>
   </si>
   <si>
-    <t>A (4)</t>
-  </si>
-  <si>
-    <t>D (4)</t>
-  </si>
-  <si>
     <t>xxxx</t>
+  </si>
+  <si>
+    <t>A (8)</t>
+  </si>
+  <si>
+    <t>D (8)</t>
+  </si>
+  <si>
+    <t>Dest (8)</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -471,10 +471,10 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -488,10 +488,10 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -508,10 +508,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -539,10 +539,10 @@
         <v>111</v>
       </c>
       <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -564,10 +564,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
         <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -581,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Put most everything together
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSCE312Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2917928D-D673-4BDC-A321-6D27F88DB423}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06435F0-B5C2-4CF1-9263-797DEBB3C6F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="2580" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Instruction</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Dest (8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,8 +580,8 @@
       <c r="C10">
         <v>1000</v>
       </c>
-      <c r="D10">
-        <v>10</v>
+      <c r="D10" t="s">
+        <v>22</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -610,6 +613,11 @@
       </c>
       <c r="D12" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>